<commit_message>
[Modified] : Statistics Rename
</commit_message>
<xml_diff>
--- a/ToDoApp-Doc/Document/Diagram/UseCase/Statistics/Statistics.xlsx
+++ b/ToDoApp-Doc/Document/Diagram/UseCase/Statistics/Statistics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\To-Do-App\ToDoApp-Doc\Document\Diagram\UseCase\Statistics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B281E3C6-E4F0-4FD7-A492-3EC2A8BF9685}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{943415E2-31FD-4764-AD36-3B250303B72A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Completed Task Statistics" sheetId="5" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="98">
   <si>
     <t>Use-case number:</t>
   </si>
@@ -39,9 +39,6 @@
     <t>Use-case name:</t>
   </si>
   <si>
-    <t>Basle course of events:</t>
-  </si>
-  <si>
     <t>Alternative paths:</t>
   </si>
   <si>
@@ -87,10 +84,6 @@
     <t>Chức năng giúp người dùng xem lại thống kê những task đã hoàn thành</t>
   </si>
   <si>
-    <t>_Lỗi mã nguồn
-_Nếu người dùng chưa từng hoàn thành task nào thì thông báo cho người dùng</t>
-  </si>
-  <si>
     <t>Người dùng muốn xem các Task đã hoàn thành</t>
   </si>
   <si>
@@ -103,20 +96,12 @@
     <t>Chức năng giúp người dùng xem lại thống kê các Achievement mà mình đã đạt được</t>
   </si>
   <si>
-    <t>_Lỗi mã nguồn
-_Nếu không tồn tại Achievement nào thì thông báo cho người dùng biết</t>
-  </si>
-  <si>
     <t>Hệ thống sẽ hiển thị danh sách thống kê Achievement ra màn hình và ở trạng thái sẵn sàng cho việc thực hiện một tác vụ khác</t>
   </si>
   <si>
     <t>Người dùng muốn xem bảng thống kê các Achievement</t>
   </si>
   <si>
-    <t>_Lỗi mã nguồn
-_Nếu chưa từng sử dụng Pomodoro trước đó hoặc sử dụng sai cách thì thông báo cho người dùng</t>
-  </si>
-  <si>
     <t>Chức năng giúp người dùng xem lại thống kê lại tần suất cũng như thời gian sử dụng app của mình</t>
   </si>
   <si>
@@ -154,10 +139,6 @@
   </si>
   <si>
     <t xml:space="preserve">Chức năng giúp người dùng xem lại thống kê các task có thời hạn </t>
-  </si>
-  <si>
-    <t>_Lỗi mã nguồn
-_Người dùng chưa từng tạo task nào trước đó hoặc tạo các task mà không có ngày hết hạn</t>
   </si>
   <si>
     <t xml:space="preserve">Người dùng muốn xem các Task có ngày hết hạn </t>
@@ -188,10 +169,6 @@
     <t>System response:</t>
   </si>
   <si>
-    <t>_Lỗi mã nguồn
-_Người dùng sử dụng app trước đó nhưng không đăng nhập</t>
-  </si>
-  <si>
     <t>Khi người dùng nhấn vào phần Account thì phải có mục Statistics xuất hiện</t>
   </si>
   <si>
@@ -216,10 +193,6 @@
     <t>Khi người dùng nhấn vào phần Task thì phải hiển thị các tag đi kèm để người dùng có thể xem</t>
   </si>
   <si>
-    <t>_Lỗi mã nguồn
-_Người dùng chưa từng sử dụng bất kì 1 loại tag nào hoặc sử dụng tag sai cách</t>
-  </si>
-  <si>
     <t>Người dùng vào Account rồi chọn phần Statistics kéo xuống sẽ thấy Tag, sau đó nhấp vào để xem bảng thống kê chi tiết</t>
   </si>
   <si>
@@ -229,20 +202,7 @@
     <t>Người dùng vào Account rồi chọn phần Statistics kéo xuống sẽ thấy Pomodoro, sau đó nhấp vào để xem bảng thống kê chi tiết</t>
   </si>
   <si>
-    <t>_Lỗi mã nguồn
-_Nếu người dùng chưa từng tạo task nào trước đó thì thông báo cho người dùng</t>
-  </si>
-  <si>
     <t>Người dùng vào Account rồi chọn phần Statistics kéo xuống sẽ thấy Task, sau đó nhấp vào để xem bảng thống kê chi tiết</t>
-  </si>
-  <si>
-    <t>Khi người dùng nhấn vào More Option ( phía trên cùng bên phải ) trong phần Task thì phải hiển thị ra các chế độ xem để người dùng có thể lựa chọn</t>
-  </si>
-  <si>
-    <t>_Người dùng nhấn vào More Option trong phần Task
-_Người dùng nhấn vào Manage Task rồi chọn phần Statistics
-_Người dùng nhấn vào View Task
-_Người dùng nhấn vào chế độ xem mình mong muốn</t>
   </si>
   <si>
     <t>_Hệ thống sẽ hiển thị danh mục các tùy chọn
@@ -251,58 +211,16 @@
 _Hệ thống sẽ đánh dấu chế độ đã được chọn và sẽ hiển thị tất cả các Task của người dùng đã tạo cũng như những chi tiết của chúng như ngày tạo, ghi chú,...được tải lên từ database hoặc local storage</t>
   </si>
   <si>
-    <t>_Người dùng nhấn vào More Option trong phần Task
-_Hệ thống sẽ hiển thị danh mục các tùy chọn
-_Người dùng nhấn vào Manage Task rồi chọn phần Statistics
-_Hệ thống sẽ hiển thị danh mục các tùy chọn khác nhau
-_Người dùng nhấn vào View Task
-_Hệ thống hiển thị các chế độ xem để người dùng có thể lựa chọn
-_Người dùng chọn các chế độ xem
-_Hệ thống sẽ đánh dấu chế độ đã được chọn và sẽ hiển thị tất cả các Task của người dùng đã tạo cũng như những chi tiết của chúng được tải lên từ database hoặc local storage</t>
-  </si>
-  <si>
-    <t>_Người dùng vào More Option trong phần Pomodoro
-_Người dùng nhấn vào Manage Pomodoro rồi chọn phần Statistics
-_Người dùng nhấn vào View 
-_Người dùng chọn các chế độ xem để xem và nhấn vào từng cái để xem chi tiết ( như ngày, giờ, thời gian bắt đầu,...)</t>
-  </si>
-  <si>
-    <t>_Người dùng vào More Option trong phần Pomodoro
-_Hệ thống sẽ hiển thị danh mục các tùy chọn
-_Người dùng nhấn vào Manage Pomodoro rồi chọn phần Statistics
-_Hệ thống sẽ hiển thị danh mục các tùy chọn khác nhau
-_Người dùng nhấn vào View 
-_Hệ thống hiển thị các chế độ xem để người dùng có thể lựa chọn
-_Người dùng chọn các chế độ xem để xem và nhấn vào từng cái để xem chi tiết ( như ngày, giờ, thời gian bắt đầu,...)
-_Hệ thống đánh dấu chế độ đã chọn và sẽ hiển thị thống kê số lần sử dụng Pomodoro của người dùng cũng như chi tiết của nó như thời gian sử dụng trung bình, số task đã hoàn thành,... được tải lên từ database hoặc local storage</t>
-  </si>
-  <si>
     <t>_Hệ thống sẽ hiển thị danh mục các tùy chọn
 _Hệ thống sẽ hiển thị danh mục các tùy chọn khác nhau
 _Hệ thống hiển thị các chế độ xem để người dùng có thể lựa chọn
 _Hệ thống đánh dấu chế độ đã chọn và sẽ hiển thị thống kê tần suất, số lần sử dụng Pomodoro của người dùng cũng như chi tiết của nó như thời gian sử dụng trung bình, số task đã hoàn thành,... được tải lên từ database hoặc local storage</t>
   </si>
   <si>
-    <t>_Người dùng vào More Option trong Achievement
-_Hệ thống sẽ hiển thị danh mục các tùy chọn
-_Người dùng nhấn vào Manage Achievement rồi chọn phần Statistics
-_Hệ thống sẽ hiển thị danh mục các tùy chọn khác nhau
-_Người dùng nhấn vào View Achievement
-_Hệ thống hiển thị các chế độ xem để người dùng có thể lựa chọn
-_Người dùng chọn các chế độ xem để xem và nhấn vào từng cái để xem chi tiết ( như ngày, giờ,...)
-_Hệ thống đánh dấu chế độ đã chọn và sẽ hiển thị tất cả các Achievement của người dùng được tải lên từ database hoặc local storage</t>
-  </si>
-  <si>
     <t>_Hệ thống sẽ hiển thị danh mục các tùy chọn
 _Hệ thống sẽ hiển thị danh mục các tùy chọn khác nhau
 _Hệ thống hiển thị các chế độ xem khác nhau để người dùng có thể lựa chọn
 _Sau đó hệ thống đánh dấu chế độ đã chọn và sẽ hiển thị danh sách thống kê các Achievement ra màn hình được tải lên từ database hoặc local storage hình để người dùng có thể xem</t>
-  </si>
-  <si>
-    <t>_Người dùng vào More Option trong Achievement
-_Người dùng nhấn vào Manage Achievement rồi chọn phần Statistics
-_Người dùng nhấn vào View Achievement
-_Người dùng chọn chế độ xem và nhấn vào từng thành phần để xem chi tiết các Achievement</t>
   </si>
   <si>
     <t>_Người dùng nhấn vào phần Task
@@ -333,13 +251,86 @@
     <t>Người dùng vào Account rồi chọn phần Statistics kéo xuống sẽ thấy Completed Task, sau đó nhấp vào để xem bảng thống kê chi tiết</t>
   </si>
   <si>
-    <t>Khi nhấn vào More Option ( phía trên cùng bên phải ) trong Task cần phải hiển thị phần Deadline Task để người dùng có thể chọn</t>
-  </si>
-  <si>
-    <t>Khi nhấn vào More Option ( phía trên cùng bên phải ) phải hiển thị phần Task Completed để người dùng có thể chọn</t>
-  </si>
-  <si>
-    <t>_Người dùng nhấn vào More Option trong phần Task
+    <t>_Hệ thống sẽ hiển thị danh mục các tùy chọn
+_Hệ thống sẽ hiển thị danh mục các tùy chọn khác nhau
+_Hệ thống sẽ hiển thị danh mục các tùy chọn
+_Hệ thống hiển thị các chế độ xem để người dùng có thể lựa chọn
+_Hệ thống sẽ đánh dấu chế độ đã được chọn
+_Hệ thống hiển thị tất cả các Task sắp đến ngày hết hạn nhưng chưa hoàn thành hoặc làm xong của người dùng cũng như những chi tiết của chúng như ngày hết hạn, ghi chú,...được tải lên từ database hoặc local storage</t>
+  </si>
+  <si>
+    <t>_Hệ thống hiển thị danh mục các tùy chọn
+_Hệ thống sẽ hiển thị danh mục các tùy chọn khác nhau
+_Hệ thống sẽ hiển thị danh mục các tùy chọn
+_Hệ thống sẽ hiển thị danh mục các chế độ xem khác nhau
+_Hệ thống sẽ đánh dấu chế độ đã được chọn và sẽ hiển thị tất cả các Task đã hoàn thành của người dùng cũng như những chi tiết của chúng như ngày hoàn thành,... được tải lên từ database hoặc local storage</t>
+  </si>
+  <si>
+    <t>_Người dùng vào Account rồi chọn phần Statistics
+_Hệ thống sẽ hiển thị danh mục các tùy chọn
+_Người dùng nhấn vào View 
+_Hệ thống hiển thị các chế độ xem để người dùng có thể lựa chọn
+_Người dùng chọn các chế độ xem khác nhau để xem và nhấn vào từng tháng hay năm để xem chi tiết về tháng hay năm đó hay có thể xem nhiều dạng biểu đồ khác nhau như biểu đồ đường, biểu đồ cột, biểu đồ tròn,...
+_Hệ thống sẽ đánh dấu chế độ đã được chọn và sẽ hiển thị thống kê số lần sử dụng App của người dùng cũng như chi tiết của nó như tần suất sử dụng, ngày sử dụng nhiều nhất,thời gian sử dụng trung bình,... được tải lên từ database hoặc local storage</t>
+  </si>
+  <si>
+    <t>_Người dùng vào Account rồi chọn phần Statistics
+_Người dùng nhấn vào View 
+_Người dùng chọn các chế độ xem khác nhau để xem và nhấn vào từng tháng hay năm để xem chi tiết về tháng hay năm đó hoặc có thể xem nhiều dạng biểu đồ khác nhau như biểu đồ đường, biểu đồ cột, biểu đồ tròn,...</t>
+  </si>
+  <si>
+    <t>_Hệ thống sẽ hiển thị danh mục các tùy chọn 
+_Hệ thống hiển thị các chế độ xem để người dùng có thể lựa chọn
+_Hệ thống sẽ đánh dấu chế độ người dùng đã được chọn và hiển thị nhiều loại biểu đồ khác nhau cũng như sẽ hiển thị thống kê số lần sử dụng App của người dùng cũng như chi tiết của nó như tần suất sử dụng, ngày sử dụng nhiều nhất,thời gian sử dụng trung bình,... được tải lên từ database hoặc local storage</t>
+  </si>
+  <si>
+    <t>UC14.1</t>
+  </si>
+  <si>
+    <t>UC14.2</t>
+  </si>
+  <si>
+    <t>UC14.3</t>
+  </si>
+  <si>
+    <t>UC14.4</t>
+  </si>
+  <si>
+    <t>UC14.5</t>
+  </si>
+  <si>
+    <t>UC14.6</t>
+  </si>
+  <si>
+    <t>UC14.7</t>
+  </si>
+  <si>
+    <t>_Người dùng nhấn vào More Actions trong phần Task
+_Hệ thống hiển thị danh mục các tùy chọn
+_Sau đó người dùng nhấn vào Manage Task rồi chọn phần Statistics
+_Hệ thống sẽ hiển thị danh mục các tùy chọn khác nhau
+_Người dùng chọn phần Completed Task
+_Hệ thống sẽ hiển thị danh mục các tùy chọn
+_Người dùng nhấn vào View Task
+_Hệ thống hiển thị các chế độ xem để người dùng có thể lựa chọn
+_Người dùng chọn các chế độ xem
+_Hệ thống sẽ đánh dấu chế độ đã được chọn và sẽ hiển thị tất cả các Task đã hoàn thành của người dùng cũng như những chi tiết của chúng được tải lên từ database hoặc local storage</t>
+  </si>
+  <si>
+    <t>_Người dùng nhấn vào More Actions trong phần Task
+_Người dùng nhấn vào Manage Task rồi chọn phần Statistics
+_Sau đó người dùng nhấn vào phần Completed Task 
+_Người dùng nhấn vào View Task
+_Người dùng chọn các chế độ xem khác nhau</t>
+  </si>
+  <si>
+    <t>Khi nhấn vào More Actions ( phía trên cùng bên phải ) phải hiển thị phần Task Completed để người dùng có thể chọn</t>
+  </si>
+  <si>
+    <t>Nếu người dùng chưa từng hoàn thành task nào thì thông báo cho người dùng</t>
+  </si>
+  <si>
+    <t>_Người dùng nhấn vào More Actions trong phần Task
 _Hệ thống sẽ hiển thị danh mục các tùy chọn
 _Sau đó người dùng nhấn vào Manage Task rồi chọn phần Statistics
 _Hệ thống sẽ hiển thị danh mục các tùy chọn khác nhau
@@ -353,7 +344,7 @@
 _Hệ thống sẽ hiển thị tất cả các Task sắp đến ngày hết hạn nhưng chưa hoàn thành của người dùng cũng như những chi tiết của chúng được tải lên từ database hoặc local storage</t>
   </si>
   <si>
-    <t>_Người dùng nhấn vào More Option trong phần Task
+    <t>_Người dùng nhấn vào More Actions trong phần Task
 _Sau đó người dùng nhấn vào Manage Task rồi chọn phần Statistics
 _Sau đó người dùng nhấn vào phần Deadline Task
 _Người dùng nhấn vào View Task
@@ -361,56 +352,79 @@
 _Hoặc người dùng có thể vào trực tiếp phần Task chọn sắp xếp theo ngày để hiển thị các Task sắp hết hạn</t>
   </si>
   <si>
-    <t>_Hệ thống sẽ hiển thị danh mục các tùy chọn
+    <t>Khi nhấn vào More Actions ( phía trên cùng bên phải ) trong Task cần phải hiển thị phần Deadline Task để người dùng có thể chọn</t>
+  </si>
+  <si>
+    <t>Người dùng chưa từng tạo task nào trước đó hoặc tạo các task mà không có ngày hết hạn</t>
+  </si>
+  <si>
+    <t>_Người dùng nhấn vào More Actions trong phần Task
+_Hệ thống sẽ hiển thị danh mục các tùy chọn
+_Người dùng nhấn vào Manage Task rồi chọn phần Statistics
 _Hệ thống sẽ hiển thị danh mục các tùy chọn khác nhau
-_Hệ thống sẽ hiển thị danh mục các tùy chọn
-_Hệ thống hiển thị các chế độ xem để người dùng có thể lựa chọn
-_Hệ thống sẽ đánh dấu chế độ đã được chọn
-_Hệ thống hiển thị tất cả các Task sắp đến ngày hết hạn nhưng chưa hoàn thành hoặc làm xong của người dùng cũng như những chi tiết của chúng như ngày hết hạn, ghi chú,...được tải lên từ database hoặc local storage</t>
-  </si>
-  <si>
-    <t>_Người dùng nhấn vào More Option trong phần Task
-_Hệ thống hiển thị danh mục các tùy chọn
-_Sau đó người dùng nhấn vào Manage Task rồi chọn phần Statistics
-_Hệ thống sẽ hiển thị danh mục các tùy chọn khác nhau
-_Người dùng chọn phần Completed Task
-_Hệ thống sẽ hiển thị danh mục các tùy chọn
 _Người dùng nhấn vào View Task
 _Hệ thống hiển thị các chế độ xem để người dùng có thể lựa chọn
 _Người dùng chọn các chế độ xem
-_Hệ thống sẽ đánh dấu chế độ đã được chọn và sẽ hiển thị tất cả các Task đã hoàn thành của người dùng cũng như những chi tiết của chúng được tải lên từ database hoặc local storage</t>
-  </si>
-  <si>
-    <t>_Hệ thống hiển thị danh mục các tùy chọn
+_Hệ thống sẽ đánh dấu chế độ đã được chọn và sẽ hiển thị tất cả các Task của người dùng đã tạo cũng như những chi tiết của chúng được tải lên từ database hoặc local storage</t>
+  </si>
+  <si>
+    <t>_Người dùng nhấn vào More Actions trong phần Task
+_Người dùng nhấn vào Manage Task rồi chọn phần Statistics
+_Người dùng nhấn vào View Task
+_Người dùng nhấn vào chế độ xem mình mong muốn</t>
+  </si>
+  <si>
+    <t>Nếu người dùng chưa từng tạo task nào trước đó thì thông báo cho người dùng</t>
+  </si>
+  <si>
+    <t>Khi người dùng nhấn vào More Actions ( phía trên cùng bên phải ) trong phần Task thì phải hiển thị ra các chế độ xem để người dùng có thể lựa chọn</t>
+  </si>
+  <si>
+    <t>Người dùng chưa từng sử dụng bất kì 1 loại tag nào hoặc sử dụng tag sai cách</t>
+  </si>
+  <si>
+    <t>_Người dùng vào More Actions trong Achievement
+_Hệ thống sẽ hiển thị danh mục các tùy chọn
+_Người dùng nhấn vào Manage Achievement rồi chọn phần Statistics
 _Hệ thống sẽ hiển thị danh mục các tùy chọn khác nhau
+_Người dùng nhấn vào View Achievement
+_Hệ thống hiển thị các chế độ xem để người dùng có thể lựa chọn
+_Người dùng chọn các chế độ xem để xem và nhấn vào từng cái để xem chi tiết ( như ngày, giờ,...)
+_Hệ thống đánh dấu chế độ đã chọn và sẽ hiển thị tất cả các Achievement của người dùng được tải lên từ database hoặc local storage</t>
+  </si>
+  <si>
+    <t>_Người dùng vào More Actions trong Achievement
+_Người dùng nhấn vào Manage Achievement rồi chọn phần Statistics
+_Người dùng nhấn vào View Achievement
+_Người dùng chọn chế độ xem và nhấn vào từng thành phần để xem chi tiết các Achievement</t>
+  </si>
+  <si>
+    <t>Nếu không tồn tại Achievement nào thì thông báo cho người dùng biết</t>
+  </si>
+  <si>
+    <t>_Người dùng vào More Actions trong phần Pomodoro
 _Hệ thống sẽ hiển thị danh mục các tùy chọn
-_Hệ thống sẽ hiển thị danh mục các chế độ xem khác nhau
-_Hệ thống sẽ đánh dấu chế độ đã được chọn và sẽ hiển thị tất cả các Task đã hoàn thành của người dùng cũng như những chi tiết của chúng như ngày hoàn thành,... được tải lên từ database hoặc local storage</t>
-  </si>
-  <si>
-    <t>_Người dùng vào Account rồi chọn phần Statistics
-_Hệ thống sẽ hiển thị danh mục các tùy chọn
+_Người dùng nhấn vào Manage Pomodoro rồi chọn phần Statistics
+_Hệ thống sẽ hiển thị danh mục các tùy chọn khác nhau
 _Người dùng nhấn vào View 
 _Hệ thống hiển thị các chế độ xem để người dùng có thể lựa chọn
-_Người dùng chọn các chế độ xem khác nhau để xem và nhấn vào từng tháng hay năm để xem chi tiết về tháng hay năm đó hay có thể xem nhiều dạng biểu đồ khác nhau như biểu đồ đường, biểu đồ cột, biểu đồ tròn,...
-_Hệ thống sẽ đánh dấu chế độ đã được chọn và sẽ hiển thị thống kê số lần sử dụng App của người dùng cũng như chi tiết của nó như tần suất sử dụng, ngày sử dụng nhiều nhất,thời gian sử dụng trung bình,... được tải lên từ database hoặc local storage</t>
-  </si>
-  <si>
-    <t>_Người dùng vào Account rồi chọn phần Statistics
+_Người dùng chọn các chế độ xem để xem và nhấn vào từng cái để xem chi tiết ( như ngày, giờ, thời gian bắt đầu,...)
+_Hệ thống đánh dấu chế độ đã chọn và sẽ hiển thị thống kê số lần sử dụng Pomodoro của người dùng cũng như chi tiết của nó như thời gian sử dụng trung bình, số task đã hoàn thành,... được tải lên từ database hoặc local storage</t>
+  </si>
+  <si>
+    <t>_Người dùng vào More Actions trong phần Pomodoro
+_Người dùng nhấn vào Manage Pomodoro rồi chọn phần Statistics
 _Người dùng nhấn vào View 
-_Người dùng chọn các chế độ xem khác nhau để xem và nhấn vào từng tháng hay năm để xem chi tiết về tháng hay năm đó hoặc có thể xem nhiều dạng biểu đồ khác nhau như biểu đồ đường, biểu đồ cột, biểu đồ tròn,...</t>
-  </si>
-  <si>
-    <t>_Hệ thống sẽ hiển thị danh mục các tùy chọn 
-_Hệ thống hiển thị các chế độ xem để người dùng có thể lựa chọn
-_Hệ thống sẽ đánh dấu chế độ người dùng đã được chọn và hiển thị nhiều loại biểu đồ khác nhau cũng như sẽ hiển thị thống kê số lần sử dụng App của người dùng cũng như chi tiết của nó như tần suất sử dụng, ngày sử dụng nhiều nhất,thời gian sử dụng trung bình,... được tải lên từ database hoặc local storage</t>
-  </si>
-  <si>
-    <t>_Người dùng nhấn vào More Option trong phần Task
-_Người dùng nhấn vào Manage Task rồi chọn phần Statistics
-_Sau đó người dùng nhấn vào phần Completed Task 
-_Người dùng nhấn vào View Task
-_Người dùng chọn các chế độ xem khác nhau</t>
+_Người dùng chọn các chế độ xem để xem và nhấn vào từng cái để xem chi tiết ( như ngày, giờ, thời gian bắt đầu,...)</t>
+  </si>
+  <si>
+    <t>Nếu chưa từng sử dụng Pomodoro trước đó hoặc sử dụng sai cách thì thông báo cho người dùng</t>
+  </si>
+  <si>
+    <t>Người dùng sử dụng app trước đó nhưng không đăng nhập</t>
+  </si>
+  <si>
+    <t>Basic course of events:</t>
   </si>
 </sst>
 </file>
@@ -805,8 +819,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C3:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -820,7 +834,9 @@
       <c r="C3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="4"/>
+      <c r="D3" s="4" t="s">
+        <v>70</v>
+      </c>
       <c r="E3" s="5"/>
     </row>
     <row r="4" spans="3:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
@@ -828,101 +844,101 @@
         <v>1</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E4" s="5"/>
     </row>
     <row r="5" spans="3:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C5" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E5" s="5"/>
     </row>
     <row r="6" spans="3:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C6" s="2" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E6" s="5"/>
     </row>
     <row r="7" spans="3:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C7" s="2" t="s">
-        <v>2</v>
+        <v>97</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="3:5" ht="238.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C8" s="3" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>86</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="3:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C9" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="E9" s="5"/>
+    </row>
+    <row r="10" spans="3:5" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C10" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="E9" s="5"/>
-    </row>
-    <row r="10" spans="3:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="2" t="s">
-        <v>4</v>
-      </c>
       <c r="D10" s="4" t="s">
-        <v>18</v>
+        <v>80</v>
       </c>
       <c r="E10" s="5"/>
     </row>
     <row r="11" spans="3:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C11" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E11" s="5"/>
     </row>
     <row r="12" spans="3:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C12" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E12" s="5"/>
     </row>
     <row r="13" spans="3:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C13" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E13" s="5"/>
     </row>
     <row r="14" spans="3:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C14" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E14" s="5"/>
     </row>
@@ -948,8 +964,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="C3:E14"/>
   <sheetViews>
-    <sheetView topLeftCell="C7" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView topLeftCell="C4" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -963,7 +979,9 @@
       <c r="C3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="4"/>
+      <c r="D3" s="4" t="s">
+        <v>71</v>
+      </c>
       <c r="E3" s="5"/>
     </row>
     <row r="4" spans="3:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
@@ -971,101 +989,101 @@
         <v>1</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E4" s="5"/>
     </row>
     <row r="5" spans="3:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C5" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E5" s="5"/>
     </row>
     <row r="6" spans="3:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C6" s="2" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="E6" s="5"/>
     </row>
     <row r="7" spans="3:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C7" s="2" t="s">
-        <v>2</v>
+        <v>97</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="3:5" ht="240" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C8" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>83</v>
-      </c>
       <c r="E8" s="3" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="3:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C9" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="E9" s="5"/>
+    </row>
+    <row r="10" spans="3:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C10" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="E9" s="5"/>
-    </row>
-    <row r="10" spans="3:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="2" t="s">
-        <v>4</v>
-      </c>
       <c r="D10" s="4" t="s">
-        <v>40</v>
+        <v>84</v>
       </c>
       <c r="E10" s="5"/>
     </row>
     <row r="11" spans="3:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C11" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="E11" s="5"/>
     </row>
     <row r="12" spans="3:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C12" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="E12" s="5"/>
     </row>
     <row r="13" spans="3:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C13" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="E13" s="5"/>
     </row>
     <row r="14" spans="3:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C14" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E14" s="5"/>
     </row>
@@ -1090,8 +1108,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="C3:E14"/>
   <sheetViews>
-    <sheetView topLeftCell="C10" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1105,7 +1123,9 @@
       <c r="C3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="4"/>
+      <c r="D3" s="4" t="s">
+        <v>72</v>
+      </c>
       <c r="E3" s="5"/>
     </row>
     <row r="4" spans="3:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
@@ -1113,101 +1133,101 @@
         <v>1</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E4" s="5"/>
     </row>
     <row r="5" spans="3:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C5" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E5" s="5"/>
     </row>
     <row r="6" spans="3:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C6" s="2" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E6" s="5"/>
     </row>
     <row r="7" spans="3:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C7" s="2" t="s">
-        <v>2</v>
+        <v>97</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="3:5" ht="158.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C8" s="3" t="s">
-        <v>68</v>
+        <v>85</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>66</v>
+        <v>86</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="3:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C9" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E9" s="5"/>
+    </row>
+    <row r="10" spans="3:5" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C10" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="E9" s="5"/>
-    </row>
-    <row r="10" spans="3:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="2" t="s">
-        <v>4</v>
-      </c>
       <c r="D10" s="4" t="s">
-        <v>63</v>
+        <v>87</v>
       </c>
       <c r="E10" s="5"/>
     </row>
     <row r="11" spans="3:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C11" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>65</v>
+        <v>88</v>
       </c>
       <c r="E11" s="5"/>
     </row>
     <row r="12" spans="3:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C12" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="E12" s="5"/>
     </row>
     <row r="13" spans="3:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C13" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E13" s="5"/>
     </row>
     <row r="14" spans="3:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C14" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="E14" s="5"/>
     </row>
@@ -1232,8 +1252,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="C3:E14"/>
   <sheetViews>
-    <sheetView topLeftCell="C7" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1247,7 +1267,9 @@
       <c r="C3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="4"/>
+      <c r="D3" s="4" t="s">
+        <v>73</v>
+      </c>
       <c r="E3" s="5"/>
     </row>
     <row r="4" spans="3:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
@@ -1255,101 +1277,101 @@
         <v>1</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E4" s="5"/>
     </row>
     <row r="5" spans="3:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C5" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E5" s="5"/>
     </row>
     <row r="6" spans="3:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C6" s="2" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E6" s="5"/>
     </row>
     <row r="7" spans="3:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C7" s="2" t="s">
-        <v>2</v>
+        <v>97</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="3:5" ht="198.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C8" s="3" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="3:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C9" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E9" s="5"/>
+    </row>
+    <row r="10" spans="3:5" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C10" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="E9" s="5"/>
-    </row>
-    <row r="10" spans="3:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="2" t="s">
-        <v>4</v>
-      </c>
       <c r="D10" s="4" t="s">
-        <v>59</v>
+        <v>89</v>
       </c>
       <c r="E10" s="5"/>
     </row>
     <row r="11" spans="3:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C11" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="E11" s="5"/>
     </row>
     <row r="12" spans="3:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C12" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E12" s="5"/>
     </row>
     <row r="13" spans="3:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C13" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="E13" s="5"/>
     </row>
     <row r="14" spans="3:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C14" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E14" s="5"/>
     </row>
@@ -1374,8 +1396,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="C3:E14"/>
   <sheetViews>
-    <sheetView topLeftCell="C11" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1389,7 +1411,9 @@
       <c r="C3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="4"/>
+      <c r="D3" s="4" t="s">
+        <v>74</v>
+      </c>
       <c r="E3" s="5"/>
     </row>
     <row r="4" spans="3:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
@@ -1397,101 +1421,101 @@
         <v>1</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E4" s="5"/>
     </row>
     <row r="5" spans="3:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C5" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E5" s="5"/>
     </row>
     <row r="6" spans="3:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C6" s="2" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E6" s="5"/>
     </row>
     <row r="7" spans="3:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C7" s="2" t="s">
-        <v>2</v>
+        <v>97</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="3:5" ht="158.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C8" s="3" t="s">
-        <v>72</v>
+        <v>90</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>74</v>
+        <v>91</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="3:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C9" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E9" s="5"/>
+    </row>
+    <row r="10" spans="3:5" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C10" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="E9" s="5"/>
-    </row>
-    <row r="10" spans="3:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="2" t="s">
-        <v>4</v>
-      </c>
       <c r="D10" s="4" t="s">
-        <v>23</v>
+        <v>92</v>
       </c>
       <c r="E10" s="5"/>
     </row>
     <row r="11" spans="3:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C11" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="E11" s="5"/>
     </row>
     <row r="12" spans="3:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C12" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E12" s="5"/>
     </row>
     <row r="13" spans="3:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C13" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="E13" s="5"/>
     </row>
     <row r="14" spans="3:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C14" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E14" s="5"/>
     </row>
@@ -1516,8 +1540,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="C3:E14"/>
   <sheetViews>
-    <sheetView topLeftCell="D11" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1531,7 +1555,9 @@
       <c r="C3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="4"/>
+      <c r="D3" s="4" t="s">
+        <v>75</v>
+      </c>
       <c r="E3" s="5"/>
     </row>
     <row r="4" spans="3:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
@@ -1539,101 +1565,101 @@
         <v>1</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E4" s="5"/>
     </row>
     <row r="5" spans="3:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C5" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E5" s="5"/>
     </row>
     <row r="6" spans="3:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C6" s="2" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="E6" s="5"/>
     </row>
     <row r="7" spans="3:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C7" s="2" t="s">
-        <v>2</v>
+        <v>97</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="3:5" ht="198.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C8" s="3" t="s">
-        <v>70</v>
+        <v>93</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>69</v>
+        <v>94</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="3:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C9" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E9" s="5"/>
+    </row>
+    <row r="10" spans="3:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C10" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="E9" s="5"/>
-    </row>
-    <row r="10" spans="3:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="2" t="s">
-        <v>4</v>
-      </c>
       <c r="D10" s="4" t="s">
-        <v>26</v>
+        <v>95</v>
       </c>
       <c r="E10" s="5"/>
     </row>
     <row r="11" spans="3:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C11" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="E11" s="5"/>
     </row>
     <row r="12" spans="3:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C12" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="E12" s="5"/>
     </row>
     <row r="13" spans="3:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C13" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="E13" s="5"/>
     </row>
     <row r="14" spans="3:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C14" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="E14" s="5"/>
     </row>
@@ -1658,8 +1684,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="C3:E14"/>
   <sheetViews>
-    <sheetView topLeftCell="C11" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1673,7 +1699,9 @@
       <c r="C3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="4"/>
+      <c r="D3" s="4" t="s">
+        <v>76</v>
+      </c>
       <c r="E3" s="5"/>
     </row>
     <row r="4" spans="3:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
@@ -1681,101 +1709,101 @@
         <v>1</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E4" s="5"/>
     </row>
     <row r="5" spans="3:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C5" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E5" s="5"/>
     </row>
     <row r="6" spans="3:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C6" s="2" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="E6" s="5"/>
     </row>
     <row r="7" spans="3:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C7" s="2" t="s">
-        <v>2</v>
+        <v>97</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="3:5" ht="236.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C8" s="3" t="s">
-        <v>87</v>
+        <v>67</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>88</v>
+        <v>68</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>89</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" spans="3:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C9" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="5"/>
+    </row>
+    <row r="10" spans="3:5" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C10" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E9" s="5"/>
-    </row>
-    <row r="10" spans="3:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="2" t="s">
+      <c r="D10" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="E10" s="5"/>
+    </row>
+    <row r="11" spans="3:5" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C11" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="E10" s="5"/>
-    </row>
-    <row r="11" spans="3:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C11" s="2" t="s">
+      <c r="D11" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E11" s="5"/>
+    </row>
+    <row r="12" spans="3:5" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C12" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="E11" s="5"/>
-    </row>
-    <row r="12" spans="3:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C12" s="2" t="s">
+      <c r="D12" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E12" s="5"/>
+    </row>
+    <row r="13" spans="3:5" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C13" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="E12" s="5"/>
-    </row>
-    <row r="13" spans="3:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="2" t="s">
-        <v>7</v>
-      </c>
       <c r="D13" s="4" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="E13" s="5"/>
     </row>
     <row r="14" spans="3:5" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C14" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E14" s="5"/>
     </row>

</xml_diff>